<commit_message>
Added 2 output features and added a column to datawide to fix 1st choice
</commit_message>
<xml_diff>
--- a/data/titleswide.xlsx
+++ b/data/titleswide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\can2c\Documents\GitHub\practicum\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B2D14C-86BD-4CB4-A625-2E4D29DFD464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A054A9-AE24-47B4-BBF5-050156FBCE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10815" yWindow="1155" windowWidth="23295" windowHeight="13575" xr2:uid="{F06E8334-0DCB-4DC1-BF96-533F5E6DBBAA}"/>
   </bookViews>
@@ -679,11 +679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A1090C-BD2C-4544-9136-CD583ECE496C}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -692,7 +692,7 @@
     <col min="5" max="16384" width="30.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -705,29 +705,30 @@
       <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="127.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -740,29 +741,30 @@
       <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="102" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -775,29 +777,30 @@
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -810,29 +813,30 @@
       <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="102" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -845,29 +849,30 @@
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -880,29 +885,30 @@
       <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -915,23 +921,24 @@
       <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -941,176 +948,179 @@
       <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="114.75" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="102" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="102" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="63.75" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="3:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" ht="51" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="3:8" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:9" ht="89.25" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="3:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:9" ht="51" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="H19" s="1" t="s">
+      <c r="F19" s="2"/>
+      <c r="I19" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="3:8" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:9" ht="63.75" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="3:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="3:8" ht="51" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:9" ht="51" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
added column title to datawide
</commit_message>
<xml_diff>
--- a/data/titleswide.xlsx
+++ b/data/titleswide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\can2c\Documents\GitHub\practicum\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A054A9-AE24-47B4-BBF5-050156FBCE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6EFB3B-E2F6-4A20-9FB4-72C8A3CEC9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10815" yWindow="1155" windowWidth="23295" windowHeight="13575" xr2:uid="{F06E8334-0DCB-4DC1-BF96-533F5E6DBBAA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
   <si>
     <t>Create and implement human centered design deliverables including but not limited to organizational change management, program implementation roadmaps, client management strategies, and more</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>Provide data/reports, analysis, and fact based guidance</t>
+  </si>
+  <si>
+    <t>Select one:</t>
   </si>
 </sst>
 </file>
@@ -705,7 +708,9 @@
       <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="F1" s="2" t="s">
         <v>40</v>
       </c>

</xml_diff>